<commit_message>
Project refactor, more backend for adding tutors.
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218DBBDD-CB2B-9242-9FE0-313674BA68EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58717A7D-8ECD-9343-94A9-549B0463EF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name:</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Began implementing backend, student creation</t>
+  </si>
+  <si>
+    <t>Restructured project. More backend for adding tutors. Worked on referential integrity of database.</t>
   </si>
 </sst>
 </file>
@@ -292,6 +295,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,9 +305,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +526,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -534,13 +537,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="20">
+      <c r="A1" s="21">
         <v>44927</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
@@ -549,19 +552,19 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="25"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
@@ -612,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="11">
         <v>44942</v>
       </c>
@@ -622,19 +625,29 @@
       <c r="C9" s="12">
         <v>0.71388888888888891</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="6"/>
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A10" s="11">
+        <v>44945</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
@@ -789,7 +802,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -798,7 +811,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>50</v>
+        <v>87.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Find tutors and show # of sessions with a student
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58717A7D-8ECD-9343-94A9-549B0463EF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C288D2D5-3EBF-1C4F-A86B-9A3979F4AA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name:</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Restructured project. More backend for adding tutors. Worked on referential integrity of database.</t>
+  </si>
+  <si>
+    <t>Generated mock data and tested tutor and student availability functionality.</t>
+  </si>
+  <si>
+    <t>Worked on a way of finding tutors available at a specific time and seeing how many times they have worked with a specific student.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -649,19 +655,39 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="6"/>
+    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A11" s="11">
+        <v>44947</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.69305555555555554</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A12" s="11">
+        <v>44948</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
@@ -802,7 +828,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>3.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -811,7 +837,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>87.5</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can view, create, delete students and tutors
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C288D2D5-3EBF-1C4F-A86B-9A3979F4AA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C26C6E-0AA9-1140-A65F-E05A58CBF871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name:</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Worked on a way of finding tutors available at a specific time and seeing how many times they have worked with a specific student.</t>
+  </si>
+  <si>
+    <t>Availability and attributes can be modified. Started adding some http response codes.</t>
+  </si>
+  <si>
+    <t>Began work on frontend interface for adding students and tutors</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -689,19 +695,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="6"/>
+    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A13" s="11">
+        <v>44954</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.46875</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="11">
+        <v>44971</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
@@ -828,7 +854,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -837,7 +863,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Info pages for edits
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C26C6E-0AA9-1140-A65F-E05A58CBF871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9325B0B6-D673-2E4D-B9E1-D4BF64AA9812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name:</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Began work on frontend interface for adding students and tutors</t>
+  </si>
+  <si>
+    <t>Added views for students and tutors in tables. Can delete both with a click. Forms to create new ones.</t>
+  </si>
+  <si>
+    <t>Student and tutor info pages to make edits and see data.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -729,19 +735,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="6"/>
+    <row r="15" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A15" s="11">
+        <v>44975</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="11">
+        <v>44976</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
@@ -854,7 +880,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>8</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -863,7 +889,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>200</v>
+        <v>287.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Session history and current availability interface
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9325B0B6-D673-2E4D-B9E1-D4BF64AA9812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABD9652-2538-D940-B35E-CBD9E1A21639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name:</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Student and tutor info pages to make edits and see data.</t>
+  </si>
+  <si>
+    <t>Support for simple queries: session history for both students and tutors, current weekly availability for both students and tutors.</t>
   </si>
 </sst>
 </file>
@@ -117,23 +120,27 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -544,7 +551,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -769,12 +776,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="6"/>
+    <row r="17" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A17" s="11">
+        <v>44977</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.46388888888888885</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5"/>
@@ -880,7 +897,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -889,7 +906,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>287.5</v>
+        <v>312.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
G Calendar availability integration for one user
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABD9652-2538-D940-B35E-CBD9E1A21639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2719F063-D788-344D-A8AE-64E09D3B8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name:</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Support for simple queries: session history for both students and tutors, current weekly availability for both students and tutors.</t>
+  </si>
+  <si>
+    <t>Began work on Google Calendar integration for availability scheduling.</t>
+  </si>
+  <si>
+    <t>Can now update availability in DB based on upcoming week's calendar events. Can also populate upcoming week in calendar with availability stored in DB. Hard-coded for one tutor.</t>
   </si>
 </sst>
 </file>
@@ -550,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -793,19 +799,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="6"/>
+    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A18" s="11">
+        <v>44982</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A19" s="11">
+        <v>44983</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
@@ -897,7 +923,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -906,7 +932,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>312.5</v>
+        <v>362.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved error handling for GCal
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2719F063-D788-344D-A8AE-64E09D3B8508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A14F8F-531B-B94E-B640-6FB966DF6ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Name:</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Can now update availability in DB based on upcoming week's calendar events. Can also populate upcoming week in calendar with availability stored in DB. Hard-coded for one tutor.</t>
+  </si>
+  <si>
+    <t>Added support for a calendar for every tutor</t>
+  </si>
+  <si>
+    <t>Improved Google Calendar multiplicity support. Error handling, etc</t>
   </si>
 </sst>
 </file>
@@ -556,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -834,18 +840,38 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="6"/>
+      <c r="A20" s="11">
+        <v>44989</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A21" s="11">
+        <v>44990</v>
+      </c>
+      <c r="B21" s="12">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
@@ -923,7 +949,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -932,7 +958,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>362.5</v>
+        <v>412.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Housekeeping, can export Student table as csv
</commit_message>
<xml_diff>
--- a/Freelance Timesheet.xlsx
+++ b/Freelance Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Documents/Tutoring Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A14F8F-531B-B94E-B640-6FB966DF6ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105981B8-CC9C-314D-8C1F-B2B888E86E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name:</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Improved Google Calendar multiplicity support. Error handling, etc</t>
+  </si>
+  <si>
+    <t>Improved upon database schema, created script to quickly reset database with mock data.</t>
+  </si>
+  <si>
+    <t>Housekeeping on student info page, can export Student table as CSV</t>
   </si>
 </sst>
 </file>
@@ -562,8 +568,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -861,10 +867,10 @@
         <v>44990</v>
       </c>
       <c r="B21" s="12">
-        <v>0.1388888888888889</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="C21" s="12">
-        <v>0.18055555555555555</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>25</v>
@@ -873,19 +879,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="6"/>
+    <row r="22" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A22" s="11">
+        <v>45013</v>
+      </c>
+      <c r="B22" s="12">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="11">
+        <v>45015</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="C23" s="12">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
@@ -949,7 +975,7 @@
       </c>
       <c r="E32" s="10">
         <f>SUM(E8:E31)</f>
-        <v>16.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="4:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -958,7 +984,7 @@
       </c>
       <c r="E33" s="10">
         <f>E32*B5</f>
-        <v>412.5</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>